<commit_message>
add http to uri
</commit_message>
<xml_diff>
--- a/esxi-hosts.xlsx
+++ b/esxi-hosts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautaonn/GIT/esxihttp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E563FEF-3A13-C749-A65F-4AC05CF2E33D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5375D629-F318-2245-8787-1E633BCDC02D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{FD2C5535-F74D-41F4-BDAC-39876CDCBDB5}"/>
   </bookViews>
@@ -167,9 +167,6 @@
     <t>01-84-7b-eb-ff-be-33</t>
   </si>
   <si>
-    <t>10.0.0.20</t>
-  </si>
-  <si>
     <t>iDRAC</t>
   </si>
   <si>
@@ -177,13 +174,16 @@
   </si>
   <si>
     <t>ESXi image</t>
+  </si>
+  <si>
+    <t>http://10.0.0.20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +201,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -223,15 +231,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -592,7 +603,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -620,8 +631,8 @@
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>43</v>
+      <c r="B1" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -647,7 +658,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>12</v>
@@ -674,7 +685,7 @@
         <v>17</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -727,7 +738,7 @@
         <v>14</v>
       </c>
       <c r="Q3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -777,7 +788,7 @@
         <v>14</v>
       </c>
       <c r="Q4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -830,7 +841,7 @@
         <v>14</v>
       </c>
       <c r="Q5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -883,7 +894,7 @@
         <v>14</v>
       </c>
       <c r="Q6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -936,15 +947,18 @@
         <v>15</v>
       </c>
       <c r="Q7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{416702FB-5DB7-C847-95FB-F3E2BF7C9E0E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>